<commit_message>
Begin plotting the imperical values vs RPM
</commit_message>
<xml_diff>
--- a/Internal Combustion Engine/Imperical Engine Calculations.xlsx
+++ b/Internal Combustion Engine/Imperical Engine Calculations.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,10 @@
     <col width="24" customWidth="1" min="9" max="9"/>
     <col width="20" customWidth="1" min="10" max="10"/>
     <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="24" customWidth="1" min="12" max="12"/>
+    <col width="19" customWidth="1" min="13" max="13"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -508,6 +512,26 @@
           <t>FFR (GPM)</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>BSFC (lb/hp-hr)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>BMEP (psi)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Brake Torque (lb-ft)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Conv Eff (%)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -543,6 +567,18 @@
       <c r="K2" s="2" t="n">
         <v>3.17006</v>
       </c>
+      <c r="L2" s="2" t="n">
+        <v>1.627338701319462e-07</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>3571445.592017488</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>0.05889514212416649</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>10.60717339913588</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -578,6 +614,18 @@
       <c r="K3" s="2" t="n">
         <v>2.113373333333334</v>
       </c>
+      <c r="L3" s="2" t="n">
+        <v>1.020315534974938e-07</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>4367109.420024044</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>0.05445450675101544</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>16.9177702311904</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -613,6 +661,18 @@
       <c r="K4" s="2" t="n">
         <v>3.17006</v>
       </c>
+      <c r="L4" s="2" t="n">
+        <v>1.458409058324653e-07</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>5180670.730124466</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>0.05055157855393314</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>11.83581772582325</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -648,6 +708,18 @@
       <c r="K5" s="2" t="n">
         <v>3.17006</v>
       </c>
+      <c r="L5" s="2" t="n">
+        <v>1.538754270174747e-07</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>5476722.326031889</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>0.04295563601340615</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>11.21781698260362</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -682,6 +754,18 @@
       </c>
       <c r="K6" s="2" t="n">
         <v>3.17006</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>1.639792824230095e-07</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>5670913.101379763</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>0.03652989827516989</v>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>10.5266125872484</v>
       </c>
     </row>
   </sheetData>
@@ -695,7 +779,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -714,6 +798,10 @@
     <col width="24" customWidth="1" min="9" max="9"/>
     <col width="19" customWidth="1" min="10" max="10"/>
     <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="22" customWidth="1" min="12" max="12"/>
+    <col width="18" customWidth="1" min="13" max="13"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -772,6 +860,26 @@
           <t>FFR (GPM)</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>BSFC (lb/hp-hr)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>BMEP (psi)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Brake Torque (lb-ft)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Conv Eff (%)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -806,6 +914,18 @@
       </c>
       <c r="K2" s="2" t="n">
         <v>2.113373333333334</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>8.24970314061121e-08</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>6105704.24351951</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>0.05957780445273425</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>20.9237393028681</v>
       </c>
     </row>
   </sheetData>
@@ -819,7 +939,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -838,6 +958,10 @@
     <col width="24" customWidth="1" min="9" max="9"/>
     <col width="20" customWidth="1" min="10" max="10"/>
     <col width="11" customWidth="1" min="11" max="11"/>
+    <col width="22" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -896,6 +1020,26 @@
           <t>FFR (GPM)</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>BSFC (lb/hp-hr)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>BMEP (psi)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Brake Torque (lb-ft)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Conv Eff (%)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -930,6 +1074,18 @@
       </c>
       <c r="K2" s="2" t="n">
         <v>3.17006</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>9.97434615114785e-08</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>7574969.834129347</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>0.07391449921475009</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>17.30585997562724</v>
       </c>
     </row>
   </sheetData>
@@ -943,7 +1099,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -962,6 +1118,10 @@
     <col width="24" customWidth="1" min="9" max="9"/>
     <col width="20" customWidth="1" min="10" max="10"/>
     <col width="19" customWidth="1" min="11" max="11"/>
+    <col width="24" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1020,6 +1180,26 @@
           <t>FFR (GPM)</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>BSFC (lb/hp-hr)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>BMEP (psi)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Brake Torque (lb-ft)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Conv Eff (%)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -1055,6 +1235,18 @@
       <c r="K2" s="2" t="n">
         <v>6.34012</v>
       </c>
+      <c r="L2" s="2" t="n">
+        <v>2.12135223575293e-07</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>5479478.16830525</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>0.0903596701038656</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>8.137009730443713</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -1090,6 +1282,18 @@
       <c r="K3" s="2" t="n">
         <v>4.226746666666667</v>
       </c>
+      <c r="L3" s="2" t="n">
+        <v>1.222584242397896e-07</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>7289198.453018753</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>0.09089071699220572</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>14.11883384834457</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -1125,6 +1329,18 @@
       <c r="K4" s="2" t="n">
         <v>4.226746666666667</v>
       </c>
+      <c r="L4" s="2" t="n">
+        <v>1.078719803728342e-07</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>9338893.621738128</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>0.09112638867029059</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>16.001804847153</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -1160,6 +1376,18 @@
       <c r="K5" s="2" t="n">
         <v>4.226746666666667</v>
       </c>
+      <c r="L5" s="2" t="n">
+        <v>1.025836179985985e-07</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>10953444.65345734</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>0.08591127203774246</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>16.82672547604623</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -1194,6 +1422,18 @@
       </c>
       <c r="K6" s="2" t="n">
         <v>5.283433333333333</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>1.228590953913845e-07</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>12614888.32776461</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>0.08126038596037537</v>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>14.04980537178086</v>
       </c>
     </row>
   </sheetData>

</xml_diff>